<commit_message>
add a "d" to inspired
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43680\Desktop\Schule\SYP\Sommerprojekt syp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06457D76-72FD-4298-BE0A-B99028EF0090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30082AB5-D3ED-4C80-AC53-9196A0A07B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="3040" windowWidth="19200" windowHeight="11170" xr2:uid="{421BF6F9-28D3-490D-AE3D-251A0DFA6C90}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{421BF6F9-28D3-490D-AE3D-251A0DFA6C90}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -104,10 +104,10 @@
     <t>Time</t>
   </si>
   <si>
-    <t>As a User, I want to get an overview on the Mainpage on how this S.T.A.L.K.E.R inspire server looks like</t>
-  </si>
-  <si>
     <t>As a User, I want to access all the information from the "About Us" section, to see why the owners choose the server to look like it actually is</t>
+  </si>
+  <si>
+    <t>As a User, I want to get an overview on the Mainpage on how this S.T.A.L.K.E.R inspired server looks like</t>
   </si>
 </sst>
 </file>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAABFAD-F519-42B9-A6C1-1F7B8DF6734D}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -531,7 +531,7 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -597,7 +597,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>

</xml_diff>